<commit_message>
solucionando problema de envio de whatsapp
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
@@ -1136,7 +1136,6 @@
           <t>10000</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -1147,16 +1146,94 @@
           <t>No pagado</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
       <c r="Y8" t="inlineStr">
         <is>
           <t>3765100571</t>
         </is>
       </c>
       <c r="Z8" t="inlineStr">
+        <is>
+          <t>3764251817</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>04/06/2025</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Ingeniero</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Físico</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Obra nueva</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>JUANI GALLO</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>FIRU LUQUE</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>FRANCISCO DE HARO 2745</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>25817/G/2025</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>151818</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>15000</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>7000</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>4000</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
         <is>
           <t>3764251817</t>
         </is>
@@ -1173,7 +1250,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1268,6 +1345,67 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>04/06/2025</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Licenciado</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Físico</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Plan de Contingencia</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>EVACUACION</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>LAUDIN JORGE</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>ARMOA ESTELA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>3764251817</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Guardado de whatsapp del profesional
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
@@ -1223,8 +1223,6 @@
           <t>4000</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -1235,11 +1233,95 @@
           <t>No pagado</t>
         </is>
       </c>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
       <c r="Y9" t="inlineStr">
+        <is>
+          <t>3764251817</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>05/06/2025</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Ingeniero</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Físico</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Obra nueva</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>VITALE JUAN ANTONIO</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>NILOS ROBERTO</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>FRANCISCO DE HARO 2745</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>1515/J/25</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>61518</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>15000</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>15000</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr">
         <is>
           <t>3764251817</t>
         </is>

</xml_diff>

<commit_message>
agregando formato a los numeros
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13605" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Obras en general" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,13 +12,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Obras en general'!$A$1:$X$68</definedName>
   </definedNames>
-  <calcPr calcId="152511" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <name val="Calibri"/>
@@ -42,7 +44,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,15 +70,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,22 +444,22 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA98"/>
+  <dimension ref="A1:AA99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col width="32.7109375" bestFit="1" customWidth="1" style="4" min="6" max="6"/>
-    <col width="49" bestFit="1" customWidth="1" style="4" min="7" max="7"/>
-    <col width="16.7109375" bestFit="1" customWidth="1" style="4" min="12" max="12"/>
-    <col width="16.140625" bestFit="1" customWidth="1" style="4" min="13" max="13"/>
-    <col width="26.5703125" bestFit="1" customWidth="1" style="4" min="14" max="14"/>
-    <col width="32.85546875" bestFit="1" customWidth="1" style="4" min="15" max="15"/>
-    <col width="28.140625" bestFit="1" customWidth="1" style="4" min="16" max="16"/>
-    <col width="35.28515625" bestFit="1" customWidth="1" style="4" min="17" max="17"/>
+    <col width="32.7109375" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
+    <col width="49" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
+    <col width="16.7109375" bestFit="1" customWidth="1" style="2" min="12" max="12"/>
+    <col width="16.140625" bestFit="1" customWidth="1" style="2" min="13" max="13"/>
+    <col width="26.5703125" bestFit="1" customWidth="1" style="2" min="14" max="14"/>
+    <col width="32.85546875" bestFit="1" customWidth="1" style="2" min="15" max="15"/>
+    <col width="28.140625" bestFit="1" customWidth="1" style="2" min="16" max="16"/>
+    <col width="35.28515625" bestFit="1" customWidth="1" style="2" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -580,17 +583,17 @@
           <t>Ruta de carpeta</t>
         </is>
       </c>
-      <c r="Y1" s="7" t="inlineStr">
+      <c r="Y1" s="5" t="inlineStr">
         <is>
           <t>WhatsApp Profesional</t>
         </is>
       </c>
-      <c r="Z1" s="7" t="inlineStr">
+      <c r="Z1" s="5" t="inlineStr">
         <is>
           <t>WhatsApp Tramitador</t>
         </is>
       </c>
-      <c r="AA1" s="7" t="inlineStr">
+      <c r="AA1" s="5" t="inlineStr">
         <is>
           <t>Analizada en Periodo</t>
         </is>
@@ -643,13 +646,16 @@
       <c r="K2" t="n">
         <v>140043</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="O2" s="2" t="n"/>
+      <c r="N2" s="6" t="n"/>
+      <c r="O2" s="6" t="n"/>
+      <c r="P2" s="6" t="n"/>
+      <c r="Q2" s="6" t="n"/>
       <c r="R2" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -733,21 +739,18 @@
       <c r="K3" t="n">
         <v>55008</v>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>146000</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>60000</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>60000</t>
-        </is>
-      </c>
+      <c r="L3" s="6" t="n">
+        <v>146000</v>
+      </c>
+      <c r="M3" s="6" t="n"/>
+      <c r="N3" s="6" t="n"/>
+      <c r="O3" s="6" t="n">
+        <v>60000</v>
+      </c>
+      <c r="P3" s="6" t="n">
+        <v>60000</v>
+      </c>
+      <c r="Q3" s="6" t="n"/>
       <c r="R3" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -831,10 +834,14 @@
       <c r="K4" t="n">
         <v>151503</v>
       </c>
-      <c r="L4" t="n">
+      <c r="L4" s="6" t="n">
         <v>16000</v>
       </c>
-      <c r="O4" s="2" t="n"/>
+      <c r="M4" s="6" t="n"/>
+      <c r="N4" s="6" t="n"/>
+      <c r="O4" s="6" t="n"/>
+      <c r="P4" s="6" t="n"/>
+      <c r="Q4" s="6" t="n"/>
       <c r="R4" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -865,7 +872,7 @@
           <t>111</t>
         </is>
       </c>
-      <c r="X4" s="5" t="inlineStr">
+      <c r="X4" s="3" t="inlineStr">
         <is>
           <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\OBRA NUEVA\INSAURRALDE BRITEZ ARIEL\IPRODHA (VIVIENDA DE AGUIRRE CRISTINA BEATRIZ)</t>
         </is>
@@ -918,18 +925,20 @@
       <c r="K5" t="n">
         <v>151879</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L5" s="6" t="n">
         <v>168000</v>
       </c>
-      <c r="M5" t="n">
+      <c r="M5" s="6" t="n">
         <v>120000</v>
       </c>
-      <c r="O5" s="3" t="n">
+      <c r="N5" s="6" t="n"/>
+      <c r="O5" s="6" t="n">
         <v>60000</v>
       </c>
-      <c r="P5" t="n">
+      <c r="P5" s="6" t="n">
         <v>60000</v>
       </c>
+      <c r="Q5" s="6" t="n"/>
       <c r="R5" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -1013,10 +1022,14 @@
       <c r="K6" t="n">
         <v>151879</v>
       </c>
-      <c r="L6" t="n">
+      <c r="L6" s="6" t="n">
         <v>43000</v>
       </c>
-      <c r="O6" s="2" t="n"/>
+      <c r="M6" s="6" t="n"/>
+      <c r="N6" s="6" t="n"/>
+      <c r="O6" s="6" t="n"/>
+      <c r="P6" s="6" t="n"/>
+      <c r="Q6" s="6" t="n"/>
       <c r="R6" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -1100,12 +1113,14 @@
       <c r="K7" t="n">
         <v>155873</v>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>110000</t>
-        </is>
-      </c>
-      <c r="O7" s="3" t="n"/>
+      <c r="L7" s="6" t="n">
+        <v>110000</v>
+      </c>
+      <c r="M7" s="6" t="n"/>
+      <c r="N7" s="6" t="n"/>
+      <c r="O7" s="6" t="n"/>
+      <c r="P7" s="6" t="n"/>
+      <c r="Q7" s="6" t="n"/>
       <c r="R7" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -1189,26 +1204,20 @@
       <c r="K8" t="n">
         <v>24289</v>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>57000</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>19000</t>
-        </is>
-      </c>
-      <c r="O8" s="3" t="inlineStr">
-        <is>
-          <t>38000</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>38000</t>
-        </is>
-      </c>
+      <c r="L8" s="6" t="n">
+        <v>57000</v>
+      </c>
+      <c r="M8" s="6" t="n"/>
+      <c r="N8" s="6" t="n">
+        <v>19000</v>
+      </c>
+      <c r="O8" s="6" t="n">
+        <v>38000</v>
+      </c>
+      <c r="P8" s="6" t="n">
+        <v>38000</v>
+      </c>
+      <c r="Q8" s="6" t="n"/>
       <c r="R8" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -1292,10 +1301,14 @@
       <c r="K9" t="n">
         <v>24289</v>
       </c>
-      <c r="L9" t="n">
+      <c r="L9" s="6" t="n">
         <v>16000</v>
       </c>
-      <c r="O9" s="3" t="n"/>
+      <c r="M9" s="6" t="n"/>
+      <c r="N9" s="6" t="n"/>
+      <c r="O9" s="6" t="n"/>
+      <c r="P9" s="6" t="n"/>
+      <c r="Q9" s="6" t="n"/>
       <c r="R9" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -1379,17 +1392,16 @@
       <c r="K10" t="n">
         <v>135007</v>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>177000</t>
-        </is>
-      </c>
-      <c r="O10" s="3" t="n"/>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
+      <c r="L10" s="6" t="n">
+        <v>177000</v>
+      </c>
+      <c r="M10" s="6" t="n"/>
+      <c r="N10" s="6" t="n"/>
+      <c r="O10" s="6" t="n"/>
+      <c r="P10" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="Q10" s="6" t="n"/>
       <c r="R10" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -1462,10 +1474,14 @@
           <t>ININM SRL</t>
         </is>
       </c>
-      <c r="L11" t="n">
+      <c r="L11" s="6" t="n">
         <v>12000</v>
       </c>
-      <c r="O11" s="3" t="n"/>
+      <c r="M11" s="6" t="n"/>
+      <c r="N11" s="6" t="n"/>
+      <c r="O11" s="6" t="n"/>
+      <c r="P11" s="6" t="n"/>
+      <c r="Q11" s="6" t="n"/>
       <c r="R11" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -1544,16 +1560,16 @@
       <c r="K12" t="n">
         <v>5542</v>
       </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>98000</t>
-        </is>
-      </c>
-      <c r="O12" s="3" t="inlineStr">
-        <is>
-          <t>48000</t>
-        </is>
-      </c>
+      <c r="L12" s="6" t="n">
+        <v>98000</v>
+      </c>
+      <c r="M12" s="6" t="n"/>
+      <c r="N12" s="6" t="n"/>
+      <c r="O12" s="6" t="n">
+        <v>48000</v>
+      </c>
+      <c r="P12" s="6" t="n"/>
+      <c r="Q12" s="6" t="n"/>
       <c r="R12" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -1637,10 +1653,14 @@
       <c r="K13" t="n">
         <v>98203</v>
       </c>
-      <c r="L13" t="n">
+      <c r="L13" s="6" t="n">
         <v>115000</v>
       </c>
-      <c r="O13" s="3" t="n"/>
+      <c r="M13" s="6" t="n"/>
+      <c r="N13" s="6" t="n"/>
+      <c r="O13" s="6" t="n"/>
+      <c r="P13" s="6" t="n"/>
+      <c r="Q13" s="6" t="n"/>
       <c r="R13" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -1724,18 +1744,20 @@
       <c r="K14" t="n">
         <v>31855</v>
       </c>
-      <c r="L14" t="n">
+      <c r="L14" s="6" t="n">
         <v>142000</v>
       </c>
-      <c r="M14" t="n">
+      <c r="M14" s="6" t="n">
         <v>95000</v>
       </c>
-      <c r="O14" s="3" t="n">
+      <c r="N14" s="6" t="n"/>
+      <c r="O14" s="6" t="n">
         <v>47500</v>
       </c>
-      <c r="P14" t="n">
+      <c r="P14" s="6" t="n">
         <v>47500</v>
       </c>
+      <c r="Q14" s="6" t="n"/>
       <c r="R14" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -1819,18 +1841,20 @@
       <c r="K15" t="n">
         <v>58831</v>
       </c>
-      <c r="L15" t="n">
+      <c r="L15" s="6" t="n">
         <v>222000</v>
       </c>
-      <c r="M15" t="n">
+      <c r="M15" s="6" t="n">
         <v>95000</v>
       </c>
-      <c r="O15" s="3" t="n">
+      <c r="N15" s="6" t="n"/>
+      <c r="O15" s="6" t="n">
         <v>48000</v>
       </c>
-      <c r="P15" t="n">
+      <c r="P15" s="6" t="n">
         <v>47000</v>
       </c>
+      <c r="Q15" s="6" t="n"/>
       <c r="R15" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -1914,10 +1938,14 @@
       <c r="K16" t="n">
         <v>58831</v>
       </c>
-      <c r="L16" t="n">
+      <c r="L16" s="6" t="n">
         <v>32000</v>
       </c>
-      <c r="O16" s="3" t="n"/>
+      <c r="M16" s="6" t="n"/>
+      <c r="N16" s="6" t="n"/>
+      <c r="O16" s="6" t="n"/>
+      <c r="P16" s="6" t="n"/>
+      <c r="Q16" s="6" t="n"/>
       <c r="R16" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -2001,18 +2029,20 @@
       <c r="K17" t="n">
         <v>41004</v>
       </c>
-      <c r="L17" t="n">
+      <c r="L17" s="6" t="n">
         <v>113000</v>
       </c>
-      <c r="N17" t="n">
+      <c r="M17" s="6" t="n"/>
+      <c r="N17" s="6" t="n">
         <v>24000</v>
       </c>
-      <c r="O17" s="3" t="n">
+      <c r="O17" s="6" t="n">
         <v>50000</v>
       </c>
-      <c r="P17" t="n">
+      <c r="P17" s="6" t="n">
         <v>50000</v>
       </c>
+      <c r="Q17" s="6" t="n"/>
       <c r="R17" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -2096,10 +2126,14 @@
       <c r="K18" t="n">
         <v>41004</v>
       </c>
-      <c r="L18" t="n">
+      <c r="L18" s="6" t="n">
         <v>31000</v>
       </c>
-      <c r="O18" s="3" t="n"/>
+      <c r="M18" s="6" t="n"/>
+      <c r="N18" s="6" t="n"/>
+      <c r="O18" s="6" t="n"/>
+      <c r="P18" s="6" t="n"/>
+      <c r="Q18" s="6" t="n"/>
       <c r="R18" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -2183,24 +2217,20 @@
       <c r="K19" t="n">
         <v>16286</v>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>208000</t>
-        </is>
-      </c>
-      <c r="M19" t="n">
+      <c r="L19" s="6" t="n">
+        <v>208000</v>
+      </c>
+      <c r="M19" s="6" t="n">
         <v>140000</v>
       </c>
-      <c r="O19" s="3" t="inlineStr">
-        <is>
-          <t>70000</t>
-        </is>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>70000</t>
-        </is>
-      </c>
+      <c r="N19" s="6" t="n"/>
+      <c r="O19" s="6" t="n">
+        <v>70000</v>
+      </c>
+      <c r="P19" s="6" t="n">
+        <v>70000</v>
+      </c>
+      <c r="Q19" s="6" t="n"/>
       <c r="R19" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -2264,10 +2294,14 @@
       <c r="K20" t="n">
         <v>16286</v>
       </c>
-      <c r="L20" t="n">
+      <c r="L20" s="6" t="n">
         <v>74000</v>
       </c>
-      <c r="O20" s="2" t="n"/>
+      <c r="M20" s="6" t="n"/>
+      <c r="N20" s="6" t="n"/>
+      <c r="O20" s="6" t="n"/>
+      <c r="P20" s="6" t="n"/>
+      <c r="Q20" s="6" t="n"/>
       <c r="R20" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -2331,10 +2365,14 @@
       <c r="K21" t="n">
         <v>72431</v>
       </c>
-      <c r="L21" t="n">
+      <c r="L21" s="6" t="n">
         <v>485000</v>
       </c>
-      <c r="O21" s="2" t="n"/>
+      <c r="M21" s="6" t="n"/>
+      <c r="N21" s="6" t="n"/>
+      <c r="O21" s="6" t="n"/>
+      <c r="P21" s="6" t="n"/>
+      <c r="Q21" s="6" t="n"/>
       <c r="R21" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -2418,10 +2456,14 @@
       <c r="K22" t="n">
         <v>7553</v>
       </c>
-      <c r="L22" t="n">
+      <c r="L22" s="6" t="n">
         <v>234000</v>
       </c>
-      <c r="O22" s="2" t="n"/>
+      <c r="M22" s="6" t="n"/>
+      <c r="N22" s="6" t="n"/>
+      <c r="O22" s="6" t="n"/>
+      <c r="P22" s="6" t="n"/>
+      <c r="Q22" s="6" t="n"/>
       <c r="R22" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -2505,12 +2547,14 @@
       <c r="K23" t="n">
         <v>96755</v>
       </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>291000</t>
-        </is>
-      </c>
-      <c r="O23" s="2" t="n"/>
+      <c r="L23" s="6" t="n">
+        <v>291000</v>
+      </c>
+      <c r="M23" s="6" t="n"/>
+      <c r="N23" s="6" t="n"/>
+      <c r="O23" s="6" t="n"/>
+      <c r="P23" s="6" t="n"/>
+      <c r="Q23" s="6" t="n"/>
       <c r="R23" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -2594,12 +2638,14 @@
       <c r="K24" t="n">
         <v>96755</v>
       </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>75000</t>
-        </is>
-      </c>
-      <c r="O24" s="2" t="n"/>
+      <c r="L24" s="6" t="n">
+        <v>75000</v>
+      </c>
+      <c r="M24" s="6" t="n"/>
+      <c r="N24" s="6" t="n"/>
+      <c r="O24" s="6" t="n"/>
+      <c r="P24" s="6" t="n"/>
+      <c r="Q24" s="6" t="n"/>
       <c r="R24" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -2683,12 +2729,14 @@
       <c r="K25" t="n">
         <v>21718</v>
       </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>18000</t>
-        </is>
-      </c>
-      <c r="O25" s="2" t="n"/>
+      <c r="L25" s="6" t="n">
+        <v>18000</v>
+      </c>
+      <c r="M25" s="6" t="n"/>
+      <c r="N25" s="6" t="n"/>
+      <c r="O25" s="6" t="n"/>
+      <c r="P25" s="6" t="n"/>
+      <c r="Q25" s="6" t="n"/>
       <c r="R25" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -2772,18 +2820,20 @@
       <c r="K26" t="n">
         <v>84762</v>
       </c>
-      <c r="L26" t="n">
+      <c r="L26" s="6" t="n">
         <v>96000</v>
       </c>
-      <c r="M26" t="n">
+      <c r="M26" s="6" t="n">
         <v>80000</v>
       </c>
-      <c r="O26" s="3" t="n">
+      <c r="N26" s="6" t="n"/>
+      <c r="O26" s="6" t="n">
         <v>40000</v>
       </c>
-      <c r="P26" t="n">
+      <c r="P26" s="6" t="n">
         <v>40000</v>
       </c>
+      <c r="Q26" s="6" t="n"/>
       <c r="R26" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -2847,12 +2897,14 @@
       <c r="K27" t="n">
         <v>149335</v>
       </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>452000</t>
-        </is>
-      </c>
-      <c r="O27" s="3" t="inlineStr"/>
+      <c r="L27" s="6" t="n">
+        <v>452000</v>
+      </c>
+      <c r="M27" s="6" t="n"/>
+      <c r="N27" s="6" t="n"/>
+      <c r="O27" s="6" t="n"/>
+      <c r="P27" s="6" t="n"/>
+      <c r="Q27" s="6" t="n"/>
       <c r="R27" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -2941,10 +2993,14 @@
       <c r="K28" t="n">
         <v>149335</v>
       </c>
-      <c r="L28" t="n">
+      <c r="L28" s="6" t="n">
         <v>101000</v>
       </c>
-      <c r="O28" s="3" t="n"/>
+      <c r="M28" s="6" t="n"/>
+      <c r="N28" s="6" t="n"/>
+      <c r="O28" s="6" t="n"/>
+      <c r="P28" s="6" t="n"/>
+      <c r="Q28" s="6" t="n"/>
       <c r="R28" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -3028,26 +3084,20 @@
       <c r="K29" t="n">
         <v>140567</v>
       </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>81000</t>
-        </is>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="O29" s="3" t="inlineStr">
-        <is>
-          <t>59000</t>
-        </is>
-      </c>
-      <c r="P29" t="inlineStr">
-        <is>
-          <t>59000</t>
-        </is>
-      </c>
+      <c r="L29" s="6" t="n">
+        <v>81000</v>
+      </c>
+      <c r="M29" s="6" t="n"/>
+      <c r="N29" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="O29" s="6" t="n">
+        <v>59000</v>
+      </c>
+      <c r="P29" s="6" t="n">
+        <v>59000</v>
+      </c>
+      <c r="Q29" s="6" t="n"/>
       <c r="R29" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -3131,10 +3181,14 @@
       <c r="K30" t="n">
         <v>140567</v>
       </c>
-      <c r="L30" t="n">
+      <c r="L30" s="6" t="n">
         <v>30000</v>
       </c>
-      <c r="O30" s="3" t="n"/>
+      <c r="M30" s="6" t="n"/>
+      <c r="N30" s="6" t="n"/>
+      <c r="O30" s="6" t="n"/>
+      <c r="P30" s="6" t="n"/>
+      <c r="Q30" s="6" t="n"/>
       <c r="R30" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -3220,18 +3274,20 @@
           <t>99984 - 99985</t>
         </is>
       </c>
-      <c r="L31" t="n">
+      <c r="L31" s="6" t="n">
         <v>52000</v>
       </c>
-      <c r="M31" t="n">
+      <c r="M31" s="6" t="n">
         <v>116000</v>
       </c>
-      <c r="O31" s="3" t="n">
+      <c r="N31" s="6" t="n"/>
+      <c r="O31" s="6" t="n">
         <v>58000</v>
       </c>
-      <c r="P31" t="n">
+      <c r="P31" s="6" t="n">
         <v>58000</v>
       </c>
+      <c r="Q31" s="6" t="n"/>
       <c r="R31" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -3317,12 +3373,14 @@
           <t>99984 - 99985</t>
         </is>
       </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>35000</t>
-        </is>
-      </c>
-      <c r="O32" s="2" t="inlineStr"/>
+      <c r="L32" s="6" t="n">
+        <v>35000</v>
+      </c>
+      <c r="M32" s="6" t="n"/>
+      <c r="N32" s="6" t="n"/>
+      <c r="O32" s="6" t="n"/>
+      <c r="P32" s="6" t="n"/>
+      <c r="Q32" s="6" t="n"/>
       <c r="R32" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -3411,10 +3469,14 @@
       <c r="K33" t="n">
         <v>153719</v>
       </c>
-      <c r="L33" t="n">
+      <c r="L33" s="6" t="n">
         <v>157000</v>
       </c>
-      <c r="O33" s="2" t="n"/>
+      <c r="M33" s="6" t="n"/>
+      <c r="N33" s="6" t="n"/>
+      <c r="O33" s="6" t="n"/>
+      <c r="P33" s="6" t="n"/>
+      <c r="Q33" s="6" t="n"/>
       <c r="R33" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -3478,21 +3540,18 @@
       <c r="K34" t="n">
         <v>86024</v>
       </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>114000</t>
-        </is>
-      </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>32000</t>
-        </is>
-      </c>
-      <c r="P34" t="inlineStr">
-        <is>
-          <t>32000</t>
-        </is>
-      </c>
+      <c r="L34" s="6" t="n">
+        <v>114000</v>
+      </c>
+      <c r="M34" s="6" t="n"/>
+      <c r="N34" s="6" t="n"/>
+      <c r="O34" s="6" t="n">
+        <v>32000</v>
+      </c>
+      <c r="P34" s="6" t="n">
+        <v>32000</v>
+      </c>
+      <c r="Q34" s="6" t="n"/>
       <c r="R34" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -3576,26 +3635,20 @@
       <c r="K35" t="n">
         <v>111410</v>
       </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>217000</t>
-        </is>
-      </c>
-      <c r="N35" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="O35" s="2" t="inlineStr">
-        <is>
-          <t>49000</t>
-        </is>
-      </c>
-      <c r="P35" t="inlineStr">
-        <is>
-          <t>49000</t>
-        </is>
-      </c>
+      <c r="L35" s="6" t="n">
+        <v>217000</v>
+      </c>
+      <c r="M35" s="6" t="n"/>
+      <c r="N35" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="O35" s="6" t="n">
+        <v>49000</v>
+      </c>
+      <c r="P35" s="6" t="n">
+        <v>49000</v>
+      </c>
+      <c r="Q35" s="6" t="n"/>
       <c r="R35" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -3679,26 +3732,20 @@
       <c r="K36" t="n">
         <v>74485</v>
       </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>111000</t>
-        </is>
-      </c>
-      <c r="N36" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="P36" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
+      <c r="L36" s="6" t="n">
+        <v>111000</v>
+      </c>
+      <c r="M36" s="6" t="n"/>
+      <c r="N36" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="O36" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="P36" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="Q36" s="6" t="n"/>
       <c r="R36" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -3782,15 +3829,18 @@
       <c r="K37" t="n">
         <v>49463</v>
       </c>
-      <c r="L37" t="n">
+      <c r="L37" s="6" t="n">
         <v>113000</v>
       </c>
-      <c r="O37" t="n">
+      <c r="M37" s="6" t="n"/>
+      <c r="N37" s="6" t="n"/>
+      <c r="O37" s="6" t="n">
         <v>24000</v>
       </c>
-      <c r="P37" t="n">
+      <c r="P37" s="6" t="n">
         <v>24000</v>
       </c>
+      <c r="Q37" s="6" t="n"/>
       <c r="R37" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -3874,26 +3924,20 @@
       <c r="K38" t="n">
         <v>33991</v>
       </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>221000</t>
-        </is>
-      </c>
-      <c r="N38" t="inlineStr">
-        <is>
-          <t>30000</t>
-        </is>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>60000</t>
-        </is>
-      </c>
-      <c r="P38" t="inlineStr">
-        <is>
-          <t>60000</t>
-        </is>
-      </c>
+      <c r="L38" s="6" t="n">
+        <v>221000</v>
+      </c>
+      <c r="M38" s="6" t="n"/>
+      <c r="N38" s="6" t="n">
+        <v>30000</v>
+      </c>
+      <c r="O38" s="6" t="n">
+        <v>60000</v>
+      </c>
+      <c r="P38" s="6" t="n">
+        <v>60000</v>
+      </c>
+      <c r="Q38" s="6" t="n"/>
       <c r="R38" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -3977,11 +4021,14 @@
       <c r="K39" t="n">
         <v>48112</v>
       </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>317000</t>
-        </is>
-      </c>
+      <c r="L39" s="6" t="n">
+        <v>317000</v>
+      </c>
+      <c r="M39" s="6" t="n"/>
+      <c r="N39" s="6" t="n"/>
+      <c r="O39" s="6" t="n"/>
+      <c r="P39" s="6" t="n"/>
+      <c r="Q39" s="6" t="n"/>
       <c r="R39" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -4065,11 +4112,14 @@
       <c r="K40" t="n">
         <v>51426</v>
       </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>136000</t>
-        </is>
-      </c>
+      <c r="L40" s="6" t="n">
+        <v>136000</v>
+      </c>
+      <c r="M40" s="6" t="n"/>
+      <c r="N40" s="6" t="n"/>
+      <c r="O40" s="6" t="n"/>
+      <c r="P40" s="6" t="n"/>
+      <c r="Q40" s="6" t="n"/>
       <c r="R40" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -4157,21 +4207,18 @@
           <t>146678</t>
         </is>
       </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>70000</t>
-        </is>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
+      <c r="L41" s="6" t="n">
+        <v>70000</v>
+      </c>
+      <c r="M41" s="6" t="n"/>
+      <c r="N41" s="6" t="n"/>
+      <c r="O41" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="P41" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="Q41" s="6" t="n"/>
       <c r="R41" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -4259,26 +4306,20 @@
           <t>146751</t>
         </is>
       </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>81000</t>
-        </is>
-      </c>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>36000</t>
-        </is>
-      </c>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t>36000</t>
-        </is>
-      </c>
+      <c r="L42" s="6" t="n">
+        <v>81000</v>
+      </c>
+      <c r="M42" s="6" t="n"/>
+      <c r="N42" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="O42" s="6" t="n">
+        <v>36000</v>
+      </c>
+      <c r="P42" s="6" t="n">
+        <v>36000</v>
+      </c>
+      <c r="Q42" s="6" t="n"/>
       <c r="R42" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -4346,21 +4387,18 @@
           <t>147.285</t>
         </is>
       </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>63000</t>
-        </is>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
+      <c r="L43" s="6" t="n">
+        <v>63000</v>
+      </c>
+      <c r="M43" s="6" t="n"/>
+      <c r="N43" s="6" t="n"/>
+      <c r="O43" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="P43" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="Q43" s="6" t="n"/>
       <c r="R43" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -4443,11 +4481,14 @@
           <t>30488</t>
         </is>
       </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>75000</t>
-        </is>
-      </c>
+      <c r="L44" s="6" t="n">
+        <v>75000</v>
+      </c>
+      <c r="M44" s="6" t="n"/>
+      <c r="N44" s="6" t="n"/>
+      <c r="O44" s="6" t="n"/>
+      <c r="P44" s="6" t="n"/>
+      <c r="Q44" s="6" t="n"/>
       <c r="R44" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -4528,11 +4569,14 @@
       <c r="K45" t="n">
         <v>150743</v>
       </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>108000</t>
-        </is>
-      </c>
+      <c r="L45" s="6" t="n">
+        <v>108000</v>
+      </c>
+      <c r="M45" s="6" t="n"/>
+      <c r="N45" s="6" t="n"/>
+      <c r="O45" s="6" t="n"/>
+      <c r="P45" s="6" t="n"/>
+      <c r="Q45" s="6" t="n"/>
       <c r="R45" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -4563,7 +4607,7 @@
           <t>112</t>
         </is>
       </c>
-      <c r="X45" s="5" t="inlineStr">
+      <c r="X45" s="3" t="inlineStr">
         <is>
           <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\REGISTRACION\CRUZ ENRIQUE EZEQUIEL\ESCALANTE CLAUDIA ELIZABETH Y PINTOS GUSTAVO JAVIER</t>
         </is>
@@ -4620,11 +4664,14 @@
           <t>147.285</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>19000</t>
-        </is>
-      </c>
+      <c r="L46" s="6" t="n">
+        <v>19000</v>
+      </c>
+      <c r="M46" s="6" t="n"/>
+      <c r="N46" s="6" t="n"/>
+      <c r="O46" s="6" t="n"/>
+      <c r="P46" s="6" t="n"/>
+      <c r="Q46" s="6" t="n"/>
       <c r="R46" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -4712,11 +4759,14 @@
           <t>42478</t>
         </is>
       </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>68000</t>
-        </is>
-      </c>
+      <c r="L47" s="6" t="n">
+        <v>68000</v>
+      </c>
+      <c r="M47" s="6" t="n"/>
+      <c r="N47" s="6" t="n"/>
+      <c r="O47" s="6" t="n"/>
+      <c r="P47" s="6" t="n"/>
+      <c r="Q47" s="6" t="n"/>
       <c r="R47" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -4804,11 +4854,14 @@
           <t>43968</t>
         </is>
       </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>136000</t>
-        </is>
-      </c>
+      <c r="L48" s="6" t="n">
+        <v>136000</v>
+      </c>
+      <c r="M48" s="6" t="n"/>
+      <c r="N48" s="6" t="n"/>
+      <c r="O48" s="6" t="n"/>
+      <c r="P48" s="6" t="n"/>
+      <c r="Q48" s="6" t="n"/>
       <c r="R48" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -4896,16 +4949,16 @@
           <t>153965</t>
         </is>
       </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>38000</t>
-        </is>
-      </c>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t>38000</t>
-        </is>
-      </c>
+      <c r="L49" s="6" t="n">
+        <v>38000</v>
+      </c>
+      <c r="M49" s="6" t="n"/>
+      <c r="N49" s="6" t="n"/>
+      <c r="O49" s="6" t="n"/>
+      <c r="P49" s="6" t="n">
+        <v>38000</v>
+      </c>
+      <c r="Q49" s="6" t="n"/>
       <c r="R49" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -4973,6 +5026,12 @@
           <t>49975</t>
         </is>
       </c>
+      <c r="L50" s="6" t="n"/>
+      <c r="M50" s="6" t="n"/>
+      <c r="N50" s="6" t="n"/>
+      <c r="O50" s="6" t="n"/>
+      <c r="P50" s="6" t="n"/>
+      <c r="Q50" s="6" t="n"/>
       <c r="R50" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -5041,11 +5100,14 @@
           <t>30504</t>
         </is>
       </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>38000</t>
-        </is>
-      </c>
+      <c r="L51" s="6" t="n">
+        <v>38000</v>
+      </c>
+      <c r="M51" s="6" t="n"/>
+      <c r="N51" s="6" t="n"/>
+      <c r="O51" s="6" t="n"/>
+      <c r="P51" s="6" t="n"/>
+      <c r="Q51" s="6" t="n"/>
       <c r="R51" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -5133,26 +5195,20 @@
           <t>25966</t>
         </is>
       </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>94000</t>
-        </is>
-      </c>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="P52" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
+      <c r="L52" s="6" t="n">
+        <v>94000</v>
+      </c>
+      <c r="M52" s="6" t="n"/>
+      <c r="N52" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="O52" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="P52" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="Q52" s="6" t="n"/>
       <c r="R52" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -5240,26 +5296,20 @@
           <t>27285</t>
         </is>
       </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>443000</t>
-        </is>
-      </c>
-      <c r="N53" t="inlineStr">
-        <is>
-          <t>50000</t>
-        </is>
-      </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>107000</t>
-        </is>
-      </c>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t>107000</t>
-        </is>
-      </c>
+      <c r="L53" s="6" t="n">
+        <v>443000</v>
+      </c>
+      <c r="M53" s="6" t="n"/>
+      <c r="N53" s="6" t="n">
+        <v>50000</v>
+      </c>
+      <c r="O53" s="6" t="n">
+        <v>107000</v>
+      </c>
+      <c r="P53" s="6" t="n">
+        <v>107000</v>
+      </c>
+      <c r="Q53" s="6" t="n"/>
       <c r="R53" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -5347,11 +5397,14 @@
           <t>147965</t>
         </is>
       </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>89000</t>
-        </is>
-      </c>
+      <c r="L54" s="6" t="n">
+        <v>89000</v>
+      </c>
+      <c r="M54" s="6" t="n"/>
+      <c r="N54" s="6" t="n"/>
+      <c r="O54" s="6" t="n"/>
+      <c r="P54" s="6" t="n"/>
+      <c r="Q54" s="6" t="n"/>
       <c r="R54" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -5434,21 +5487,18 @@
           <t>08617</t>
         </is>
       </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>175000</t>
-        </is>
-      </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>47000</t>
-        </is>
-      </c>
-      <c r="P55" t="inlineStr">
-        <is>
-          <t>40000</t>
-        </is>
-      </c>
+      <c r="L55" s="6" t="n">
+        <v>175000</v>
+      </c>
+      <c r="M55" s="6" t="n"/>
+      <c r="N55" s="6" t="n"/>
+      <c r="O55" s="6" t="n">
+        <v>47000</v>
+      </c>
+      <c r="P55" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="Q55" s="6" t="n"/>
       <c r="R55" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -5531,11 +5581,14 @@
           <t>41282</t>
         </is>
       </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>38400</t>
-        </is>
-      </c>
+      <c r="L56" s="6" t="n">
+        <v>38400</v>
+      </c>
+      <c r="M56" s="6" t="n"/>
+      <c r="N56" s="6" t="n"/>
+      <c r="O56" s="6" t="n"/>
+      <c r="P56" s="6" t="n"/>
+      <c r="Q56" s="6" t="n"/>
       <c r="R56" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -5613,11 +5666,14 @@
           <t>41282</t>
         </is>
       </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>30000</t>
-        </is>
-      </c>
+      <c r="L57" s="6" t="n">
+        <v>30000</v>
+      </c>
+      <c r="M57" s="6" t="n"/>
+      <c r="N57" s="6" t="n"/>
+      <c r="O57" s="6" t="n"/>
+      <c r="P57" s="6" t="n"/>
+      <c r="Q57" s="6" t="n"/>
       <c r="R57" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -5700,21 +5756,18 @@
           <t>029535</t>
         </is>
       </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>170000</t>
-        </is>
-      </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>47000</t>
-        </is>
-      </c>
-      <c r="P58" t="inlineStr">
-        <is>
-          <t>47000</t>
-        </is>
-      </c>
+      <c r="L58" s="6" t="n">
+        <v>170000</v>
+      </c>
+      <c r="M58" s="6" t="n"/>
+      <c r="N58" s="6" t="n"/>
+      <c r="O58" s="6" t="n">
+        <v>47000</v>
+      </c>
+      <c r="P58" s="6" t="n">
+        <v>47000</v>
+      </c>
+      <c r="Q58" s="6" t="n"/>
       <c r="R58" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -5745,7 +5798,7 @@
           <t>112</t>
         </is>
       </c>
-      <c r="X58" s="5" t="inlineStr">
+      <c r="X58" s="3" t="inlineStr">
         <is>
           <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\REGISTRACION\ENRIQUEZ RICARDO JOSE\CANTERO LUIS ALBERTO Y ELISA LUISA BELARDINELLI</t>
         </is>
@@ -5802,11 +5855,14 @@
           <t>142496</t>
         </is>
       </c>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>126000</t>
-        </is>
-      </c>
+      <c r="L59" s="6" t="n">
+        <v>126000</v>
+      </c>
+      <c r="M59" s="6" t="n"/>
+      <c r="N59" s="6" t="n"/>
+      <c r="O59" s="6" t="n"/>
+      <c r="P59" s="6" t="n"/>
+      <c r="Q59" s="6" t="n"/>
       <c r="R59" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -5872,11 +5928,14 @@
       <c r="K60" t="n">
         <v>151503</v>
       </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>15000</t>
-        </is>
-      </c>
+      <c r="L60" s="6" t="n">
+        <v>15000</v>
+      </c>
+      <c r="M60" s="6" t="n"/>
+      <c r="N60" s="6" t="n"/>
+      <c r="O60" s="6" t="n"/>
+      <c r="P60" s="6" t="n"/>
+      <c r="Q60" s="6" t="n"/>
       <c r="R60" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -5907,7 +5966,7 @@
           <t>112</t>
         </is>
       </c>
-      <c r="X60" s="5" t="inlineStr">
+      <c r="X60" s="3" t="inlineStr">
         <is>
           <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\REGISTRACION\INSAURRALDE BRITEZ ARIEL\IPRODHA (VIVIENDA DE AGUIRRE CRISTINA BEATRIZ) 2</t>
         </is>
@@ -5964,11 +6023,14 @@
           <t>6.687</t>
         </is>
       </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>103000</t>
-        </is>
-      </c>
+      <c r="L61" s="6" t="n">
+        <v>103000</v>
+      </c>
+      <c r="M61" s="6" t="n"/>
+      <c r="N61" s="6" t="n"/>
+      <c r="O61" s="6" t="n"/>
+      <c r="P61" s="6" t="n"/>
+      <c r="Q61" s="6" t="n"/>
       <c r="R61" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -6056,11 +6118,14 @@
           <t>29839</t>
         </is>
       </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>93000</t>
-        </is>
-      </c>
+      <c r="L62" s="6" t="n">
+        <v>93000</v>
+      </c>
+      <c r="M62" s="6" t="n"/>
+      <c r="N62" s="6" t="n"/>
+      <c r="O62" s="6" t="n"/>
+      <c r="P62" s="6" t="n"/>
+      <c r="Q62" s="6" t="n"/>
       <c r="R62" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -6148,21 +6213,18 @@
           <t>137683</t>
         </is>
       </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>75000</t>
-        </is>
-      </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>30000</t>
-        </is>
-      </c>
-      <c r="P63" t="inlineStr">
-        <is>
-          <t>30000</t>
-        </is>
-      </c>
+      <c r="L63" s="6" t="n">
+        <v>75000</v>
+      </c>
+      <c r="M63" s="6" t="n"/>
+      <c r="N63" s="6" t="n"/>
+      <c r="O63" s="6" t="n">
+        <v>30000</v>
+      </c>
+      <c r="P63" s="6" t="n">
+        <v>30000</v>
+      </c>
+      <c r="Q63" s="6" t="n"/>
       <c r="R63" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -6250,6 +6312,12 @@
           <t>137683</t>
         </is>
       </c>
+      <c r="L64" s="6" t="n"/>
+      <c r="M64" s="6" t="n"/>
+      <c r="N64" s="6" t="n"/>
+      <c r="O64" s="6" t="n"/>
+      <c r="P64" s="6" t="n"/>
+      <c r="Q64" s="6" t="n"/>
       <c r="R64" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -6337,21 +6405,18 @@
           <t>152363</t>
         </is>
       </c>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>103000</t>
-        </is>
-      </c>
-      <c r="O65" t="inlineStr">
-        <is>
-          <t>40000</t>
-        </is>
-      </c>
-      <c r="P65" t="inlineStr">
-        <is>
-          <t>40000</t>
-        </is>
-      </c>
+      <c r="L65" s="6" t="n">
+        <v>103000</v>
+      </c>
+      <c r="M65" s="6" t="n"/>
+      <c r="N65" s="6" t="n"/>
+      <c r="O65" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="P65" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="Q65" s="6" t="n"/>
       <c r="R65" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -6417,25 +6482,19 @@
           <t>87107</t>
         </is>
       </c>
-      <c r="L66" t="inlineStr">
-        <is>
-          <t>119000</t>
-        </is>
-      </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>47000</t>
-        </is>
-      </c>
-      <c r="P66" t="inlineStr">
-        <is>
-          <t>47000</t>
-        </is>
-      </c>
-      <c r="Q66" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
+      <c r="L66" s="6" t="n">
+        <v>119000</v>
+      </c>
+      <c r="M66" s="6" t="n"/>
+      <c r="N66" s="6" t="n"/>
+      <c r="O66" s="6" t="n">
+        <v>47000</v>
+      </c>
+      <c r="P66" s="6" t="n">
+        <v>47000</v>
+      </c>
+      <c r="Q66" s="6" t="n">
+        <v>24000</v>
       </c>
       <c r="R66" t="inlineStr">
         <is>
@@ -6467,7 +6526,7 @@
           <t>112</t>
         </is>
       </c>
-      <c r="X66" s="5" t="inlineStr">
+      <c r="X66" s="3" t="inlineStr">
         <is>
           <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\REGISTRACION\ACEVEDO FRANCO IVAN\VILLALBA AYALA NICOLAS QUINTIN</t>
         </is>
@@ -6524,21 +6583,18 @@
           <t>9708</t>
         </is>
       </c>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>789000</t>
-        </is>
-      </c>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>130000</t>
-        </is>
-      </c>
-      <c r="P67" t="inlineStr">
-        <is>
-          <t>20000</t>
-        </is>
-      </c>
+      <c r="L67" s="6" t="n">
+        <v>789000</v>
+      </c>
+      <c r="M67" s="6" t="n"/>
+      <c r="N67" s="6" t="n"/>
+      <c r="O67" s="6" t="n">
+        <v>130000</v>
+      </c>
+      <c r="P67" s="6" t="n">
+        <v>20000</v>
+      </c>
+      <c r="Q67" s="6" t="n"/>
       <c r="R67" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -6626,21 +6682,18 @@
           <t>152369</t>
         </is>
       </c>
-      <c r="L68" t="inlineStr">
-        <is>
-          <t>186000</t>
-        </is>
-      </c>
-      <c r="O68" t="inlineStr">
-        <is>
-          <t>48000</t>
-        </is>
-      </c>
-      <c r="P68" t="inlineStr">
-        <is>
-          <t>48000</t>
-        </is>
-      </c>
+      <c r="L68" s="6" t="n">
+        <v>186000</v>
+      </c>
+      <c r="M68" s="6" t="n"/>
+      <c r="N68" s="6" t="n"/>
+      <c r="O68" s="6" t="n">
+        <v>48000</v>
+      </c>
+      <c r="P68" s="6" t="n">
+        <v>48000</v>
+      </c>
+      <c r="Q68" s="6" t="n"/>
       <c r="R68" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -6671,7 +6724,7 @@
           <t>112</t>
         </is>
       </c>
-      <c r="X68" s="5" t="inlineStr">
+      <c r="X68" s="3" t="inlineStr">
         <is>
           <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\REGISTRACION\OUDIN HUGO ORLANDO\FAYFER VIVIANA LETIZIA</t>
         </is>
@@ -6728,21 +6781,18 @@
           <t>119565</t>
         </is>
       </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>231000</t>
-        </is>
-      </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>47000</t>
-        </is>
-      </c>
-      <c r="P69" t="inlineStr">
-        <is>
-          <t>47000</t>
-        </is>
-      </c>
+      <c r="L69" s="6" t="n">
+        <v>231000</v>
+      </c>
+      <c r="M69" s="6" t="n"/>
+      <c r="N69" s="6" t="n"/>
+      <c r="O69" s="6" t="n">
+        <v>47000</v>
+      </c>
+      <c r="P69" s="6" t="n">
+        <v>47000</v>
+      </c>
+      <c r="Q69" s="6" t="n"/>
       <c r="R69" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -6810,26 +6860,20 @@
           <t>140876</t>
         </is>
       </c>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>129000</t>
-        </is>
-      </c>
-      <c r="N70" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>68000</t>
-        </is>
-      </c>
-      <c r="P70" t="inlineStr">
-        <is>
-          <t>68000</t>
-        </is>
-      </c>
+      <c r="L70" s="6" t="n">
+        <v>129000</v>
+      </c>
+      <c r="M70" s="6" t="n"/>
+      <c r="N70" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="O70" s="6" t="n">
+        <v>68000</v>
+      </c>
+      <c r="P70" s="6" t="n">
+        <v>68000</v>
+      </c>
+      <c r="Q70" s="6" t="n"/>
       <c r="R70" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -6917,11 +6961,14 @@
           <t>140876</t>
         </is>
       </c>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>31000</t>
-        </is>
-      </c>
+      <c r="L71" s="6" t="n">
+        <v>31000</v>
+      </c>
+      <c r="M71" s="6" t="n"/>
+      <c r="N71" s="6" t="n"/>
+      <c r="O71" s="6" t="n"/>
+      <c r="P71" s="6" t="n"/>
+      <c r="Q71" s="6" t="n"/>
       <c r="R71" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -7009,26 +7056,20 @@
           <t>105814</t>
         </is>
       </c>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>59000</t>
-        </is>
-      </c>
-      <c r="N72" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="P72" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
+      <c r="L72" s="6" t="n">
+        <v>59000</v>
+      </c>
+      <c r="M72" s="6" t="n"/>
+      <c r="N72" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="O72" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="P72" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="Q72" s="6" t="n"/>
       <c r="R72" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -7059,7 +7100,7 @@
           <t>112</t>
         </is>
       </c>
-      <c r="X72" s="5" t="inlineStr">
+      <c r="X72" s="3" t="inlineStr">
         <is>
           <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\REGISTRACION\FLORENTIN ALEJANDRO DANIEL\ROMERO GERTRUDIS GRACIELA</t>
         </is>
@@ -7116,21 +7157,18 @@
           <t>102426</t>
         </is>
       </c>
-      <c r="L73" t="inlineStr">
-        <is>
-          <t>219000</t>
-        </is>
-      </c>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>48000</t>
-        </is>
-      </c>
-      <c r="P73" t="inlineStr">
-        <is>
-          <t>48000</t>
-        </is>
-      </c>
+      <c r="L73" s="6" t="n">
+        <v>219000</v>
+      </c>
+      <c r="M73" s="6" t="n"/>
+      <c r="N73" s="6" t="n"/>
+      <c r="O73" s="6" t="n">
+        <v>48000</v>
+      </c>
+      <c r="P73" s="6" t="n">
+        <v>48000</v>
+      </c>
+      <c r="Q73" s="6" t="n"/>
       <c r="R73" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -7161,7 +7199,7 @@
           <t>112</t>
         </is>
       </c>
-      <c r="X73" s="5" t="inlineStr">
+      <c r="X73" s="3" t="inlineStr">
         <is>
           <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\REGISTRACION\PIZARRO JUAN MARIANO\FLORENTIN EDITH MAGDALENA</t>
         </is>
@@ -7218,21 +7256,18 @@
           <t>112258</t>
         </is>
       </c>
-      <c r="L74" t="inlineStr">
-        <is>
-          <t>36000</t>
-        </is>
-      </c>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="P74" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
+      <c r="L74" s="6" t="n">
+        <v>36000</v>
+      </c>
+      <c r="M74" s="6" t="n"/>
+      <c r="N74" s="6" t="n"/>
+      <c r="O74" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="P74" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="Q74" s="6" t="n"/>
       <c r="R74" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -7320,21 +7355,18 @@
           <t>35375</t>
         </is>
       </c>
-      <c r="L75" t="inlineStr">
-        <is>
-          <t>36000</t>
-        </is>
-      </c>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="P75" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
+      <c r="L75" s="6" t="n">
+        <v>36000</v>
+      </c>
+      <c r="M75" s="6" t="n"/>
+      <c r="N75" s="6" t="n"/>
+      <c r="O75" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="P75" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="Q75" s="6" t="n"/>
       <c r="R75" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -7422,6 +7454,12 @@
           <t>52870</t>
         </is>
       </c>
+      <c r="L76" s="6" t="n"/>
+      <c r="M76" s="6" t="n"/>
+      <c r="N76" s="6" t="n"/>
+      <c r="O76" s="6" t="n"/>
+      <c r="P76" s="6" t="n"/>
+      <c r="Q76" s="6" t="n"/>
       <c r="R76" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -7489,6 +7527,12 @@
           <t>52870</t>
         </is>
       </c>
+      <c r="L77" s="6" t="n"/>
+      <c r="M77" s="6" t="n"/>
+      <c r="N77" s="6" t="n"/>
+      <c r="O77" s="6" t="n"/>
+      <c r="P77" s="6" t="n"/>
+      <c r="Q77" s="6" t="n"/>
       <c r="R77" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -7556,11 +7600,14 @@
           <t>144880</t>
         </is>
       </c>
-      <c r="L78" t="inlineStr">
-        <is>
-          <t>30000</t>
-        </is>
-      </c>
+      <c r="L78" s="6" t="n">
+        <v>30000</v>
+      </c>
+      <c r="M78" s="6" t="n"/>
+      <c r="N78" s="6" t="n"/>
+      <c r="O78" s="6" t="n"/>
+      <c r="P78" s="6" t="n"/>
+      <c r="Q78" s="6" t="n"/>
       <c r="R78" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -7648,11 +7695,14 @@
           <t>105745</t>
         </is>
       </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>81000</t>
-        </is>
-      </c>
+      <c r="L79" s="6" t="n">
+        <v>81000</v>
+      </c>
+      <c r="M79" s="6" t="n"/>
+      <c r="N79" s="6" t="n"/>
+      <c r="O79" s="6" t="n"/>
+      <c r="P79" s="6" t="n"/>
+      <c r="Q79" s="6" t="n"/>
       <c r="R79" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -7735,11 +7785,14 @@
           <t>40210</t>
         </is>
       </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>149000</t>
-        </is>
-      </c>
+      <c r="L80" s="6" t="n">
+        <v>149000</v>
+      </c>
+      <c r="M80" s="6" t="n"/>
+      <c r="N80" s="6" t="n"/>
+      <c r="O80" s="6" t="n"/>
+      <c r="P80" s="6" t="n"/>
+      <c r="Q80" s="6" t="n"/>
       <c r="R80" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -7827,11 +7880,14 @@
           <t>135.118 AL 135.127</t>
         </is>
       </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>590000</t>
-        </is>
-      </c>
+      <c r="L81" s="6" t="n">
+        <v>590000</v>
+      </c>
+      <c r="M81" s="6" t="n"/>
+      <c r="N81" s="6" t="n"/>
+      <c r="O81" s="6" t="n"/>
+      <c r="P81" s="6" t="n"/>
+      <c r="Q81" s="6" t="n"/>
       <c r="R81" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -7919,11 +7975,14 @@
           <t>8355</t>
         </is>
       </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>31000</t>
-        </is>
-      </c>
+      <c r="L82" s="6" t="n">
+        <v>31000</v>
+      </c>
+      <c r="M82" s="6" t="n"/>
+      <c r="N82" s="6" t="n"/>
+      <c r="O82" s="6" t="n"/>
+      <c r="P82" s="6" t="n"/>
+      <c r="Q82" s="6" t="n"/>
       <c r="R82" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -7991,11 +8050,14 @@
           <t>146472</t>
         </is>
       </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>55000</t>
-        </is>
-      </c>
+      <c r="L83" s="6" t="n">
+        <v>55000</v>
+      </c>
+      <c r="M83" s="6" t="n"/>
+      <c r="N83" s="6" t="n"/>
+      <c r="O83" s="6" t="n"/>
+      <c r="P83" s="6" t="n"/>
+      <c r="Q83" s="6" t="n"/>
       <c r="R83" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8006,7 +8068,7 @@
           <t>No pagado</t>
         </is>
       </c>
-      <c r="X83" s="5" t="inlineStr">
+      <c r="X83" s="3" t="inlineStr">
         <is>
           <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\OBRA NUEVA\SILKE ADRIANO NAHUEL\LEIVA MARCELO RAUL</t>
         </is>
@@ -8063,11 +8125,14 @@
           <t>140728</t>
         </is>
       </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>26000</t>
-        </is>
-      </c>
+      <c r="L84" s="6" t="n">
+        <v>26000</v>
+      </c>
+      <c r="M84" s="6" t="n"/>
+      <c r="N84" s="6" t="n"/>
+      <c r="O84" s="6" t="n"/>
+      <c r="P84" s="6" t="n"/>
+      <c r="Q84" s="6" t="n"/>
       <c r="R84" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8135,16 +8200,16 @@
           <t>146220</t>
         </is>
       </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>190000</t>
-        </is>
-      </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>48000</t>
-        </is>
-      </c>
+      <c r="L85" s="6" t="n">
+        <v>190000</v>
+      </c>
+      <c r="M85" s="6" t="n"/>
+      <c r="N85" s="6" t="n"/>
+      <c r="O85" s="6" t="n">
+        <v>48000</v>
+      </c>
+      <c r="P85" s="6" t="n"/>
+      <c r="Q85" s="6" t="n"/>
       <c r="R85" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8155,7 +8220,7 @@
           <t>No pagado</t>
         </is>
       </c>
-      <c r="X85" s="5" t="inlineStr">
+      <c r="X85" s="3" t="inlineStr">
         <is>
           <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\REGISTRACION\ZARATE VICTOR GERONIMO\SZCZERBATIUK FEDERICO ALEJANDRO</t>
         </is>
@@ -8212,21 +8277,18 @@
           <t>142868</t>
         </is>
       </c>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>107000</t>
-        </is>
-      </c>
-      <c r="O86" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
-      <c r="P86" t="inlineStr">
-        <is>
-          <t>24000</t>
-        </is>
-      </c>
+      <c r="L86" s="6" t="n">
+        <v>107000</v>
+      </c>
+      <c r="M86" s="6" t="n"/>
+      <c r="N86" s="6" t="n"/>
+      <c r="O86" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="P86" s="6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="Q86" s="6" t="n"/>
       <c r="R86" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8294,11 +8356,14 @@
           <t>21.146</t>
         </is>
       </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>218000</t>
-        </is>
-      </c>
+      <c r="L87" s="6" t="n">
+        <v>218000</v>
+      </c>
+      <c r="M87" s="6" t="n"/>
+      <c r="N87" s="6" t="n"/>
+      <c r="O87" s="6" t="n"/>
+      <c r="P87" s="6" t="n"/>
+      <c r="Q87" s="6" t="n"/>
       <c r="R87" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8366,6 +8431,12 @@
           <t>142868</t>
         </is>
       </c>
+      <c r="L88" s="6" t="n"/>
+      <c r="M88" s="6" t="n"/>
+      <c r="N88" s="6" t="n"/>
+      <c r="O88" s="6" t="n"/>
+      <c r="P88" s="6" t="n"/>
+      <c r="Q88" s="6" t="n"/>
       <c r="R88" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8433,11 +8504,14 @@
           <t>992</t>
         </is>
       </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>56000</t>
-        </is>
-      </c>
+      <c r="L89" s="6" t="n">
+        <v>56000</v>
+      </c>
+      <c r="M89" s="6" t="n"/>
+      <c r="N89" s="6" t="n"/>
+      <c r="O89" s="6" t="n"/>
+      <c r="P89" s="6" t="n"/>
+      <c r="Q89" s="6" t="n"/>
       <c r="R89" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8500,6 +8574,12 @@
           <t>992</t>
         </is>
       </c>
+      <c r="L90" s="6" t="n"/>
+      <c r="M90" s="6" t="n"/>
+      <c r="N90" s="6" t="n"/>
+      <c r="O90" s="6" t="n"/>
+      <c r="P90" s="6" t="n"/>
+      <c r="Q90" s="6" t="n"/>
       <c r="R90" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8562,11 +8642,14 @@
           <t>63305</t>
         </is>
       </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>28000</t>
-        </is>
-      </c>
+      <c r="L91" s="6" t="n">
+        <v>28000</v>
+      </c>
+      <c r="M91" s="6" t="n"/>
+      <c r="N91" s="6" t="n"/>
+      <c r="O91" s="6" t="n"/>
+      <c r="P91" s="6" t="n"/>
+      <c r="Q91" s="6" t="n"/>
       <c r="R91" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8629,6 +8712,12 @@
           <t>63305</t>
         </is>
       </c>
+      <c r="L92" s="6" t="n"/>
+      <c r="M92" s="6" t="n"/>
+      <c r="N92" s="6" t="n"/>
+      <c r="O92" s="6" t="n"/>
+      <c r="P92" s="6" t="n"/>
+      <c r="Q92" s="6" t="n"/>
       <c r="R92" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8691,11 +8780,14 @@
           <t>59140</t>
         </is>
       </c>
-      <c r="L93" t="inlineStr">
-        <is>
-          <t>71000</t>
-        </is>
-      </c>
+      <c r="L93" s="6" t="n">
+        <v>71000</v>
+      </c>
+      <c r="M93" s="6" t="n"/>
+      <c r="N93" s="6" t="n"/>
+      <c r="O93" s="6" t="n"/>
+      <c r="P93" s="6" t="n"/>
+      <c r="Q93" s="6" t="n"/>
       <c r="R93" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8758,6 +8850,12 @@
           <t>4418</t>
         </is>
       </c>
+      <c r="L94" s="6" t="n"/>
+      <c r="M94" s="6" t="n"/>
+      <c r="N94" s="6" t="n"/>
+      <c r="O94" s="6" t="n"/>
+      <c r="P94" s="6" t="n"/>
+      <c r="Q94" s="6" t="n"/>
       <c r="R94" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8825,11 +8923,14 @@
           <t>2746</t>
         </is>
       </c>
-      <c r="L95" t="inlineStr">
-        <is>
-          <t>16000</t>
-        </is>
-      </c>
+      <c r="L95" s="6" t="n">
+        <v>16000</v>
+      </c>
+      <c r="M95" s="6" t="n"/>
+      <c r="N95" s="6" t="n"/>
+      <c r="O95" s="6" t="n"/>
+      <c r="P95" s="6" t="n"/>
+      <c r="Q95" s="6" t="n"/>
       <c r="R95" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8892,21 +8993,18 @@
           <t>21658</t>
         </is>
       </c>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>255000</t>
-        </is>
-      </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>59000</t>
-        </is>
-      </c>
-      <c r="P96" t="inlineStr">
-        <is>
-          <t>59000</t>
-        </is>
-      </c>
+      <c r="L96" s="6" t="n">
+        <v>255000</v>
+      </c>
+      <c r="M96" s="6" t="n"/>
+      <c r="N96" s="6" t="n"/>
+      <c r="O96" s="6" t="n">
+        <v>59000</v>
+      </c>
+      <c r="P96" s="6" t="n">
+        <v>59000</v>
+      </c>
+      <c r="Q96" s="6" t="n"/>
       <c r="R96" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8917,7 +9015,7 @@
           <t>No pagado</t>
         </is>
       </c>
-      <c r="X96" s="5" t="inlineStr">
+      <c r="X96" s="3" t="inlineStr">
         <is>
           <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\OBRA NUEVA\FARIAS OSVALDO\FARIAS LUCIANO OSVALDO</t>
         </is>
@@ -8974,6 +9072,12 @@
           <t>22090</t>
         </is>
       </c>
+      <c r="L97" s="6" t="n"/>
+      <c r="M97" s="6" t="n"/>
+      <c r="N97" s="6" t="n"/>
+      <c r="O97" s="6" t="n"/>
+      <c r="P97" s="6" t="n"/>
+      <c r="Q97" s="6" t="n"/>
       <c r="R97" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -9041,6 +9145,12 @@
           <t>16465</t>
         </is>
       </c>
+      <c r="L98" s="6" t="n"/>
+      <c r="M98" s="6" t="n"/>
+      <c r="N98" s="6" t="n"/>
+      <c r="O98" s="6" t="n"/>
+      <c r="P98" s="6" t="n"/>
+      <c r="Q98" s="6" t="n"/>
       <c r="R98" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -9056,6 +9166,115 @@
           <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\REGISTRACION\EDSBERG IVAN\CORTES MARIA DANIELLA</t>
         </is>
       </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>07/06/2025</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Ingeniero</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Físico</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Registración</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>DE JESUS ABIGAIL</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>ALARCON BRIAN</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>CHACRA 251 CALLE 2</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>1515/D/2024</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>15151</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>18000.0</t>
+        </is>
+      </c>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>2000.0</t>
+        </is>
+      </c>
+      <c r="P99" t="inlineStr">
+        <is>
+          <t>7000.0</t>
+        </is>
+      </c>
+      <c r="Q99" t="inlineStr"/>
+      <c r="R99" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="S99" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="T99" t="inlineStr">
+        <is>
+          <t>9999</t>
+        </is>
+      </c>
+      <c r="U99" t="inlineStr">
+        <is>
+          <t>07/06/2025</t>
+        </is>
+      </c>
+      <c r="V99" t="inlineStr">
+        <is>
+          <t>MUNI DIGITAL</t>
+        </is>
+      </c>
+      <c r="W99" t="inlineStr">
+        <is>
+          <t>112</t>
+        </is>
+      </c>
+      <c r="Y99" t="inlineStr">
+        <is>
+          <t>3764251817</t>
+        </is>
+      </c>
+      <c r="Z99" t="inlineStr"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:X68"/>
@@ -9091,7 +9310,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col width="9.7109375" bestFit="1" customWidth="1" style="4" min="12" max="12"/>
+    <col width="9.7109375" bestFit="1" customWidth="1" style="2" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -9170,12 +9389,12 @@
           <t>Ruta de carpeta</t>
         </is>
       </c>
-      <c r="P1" s="7" t="inlineStr">
+      <c r="P1" s="5" t="inlineStr">
         <is>
           <t>WhatsApp Profesional</t>
         </is>
       </c>
-      <c r="Q1" s="7" t="inlineStr">
+      <c r="Q1" s="5" t="inlineStr">
         <is>
           <t>WhatsApp Tramitador</t>
         </is>
@@ -10384,7 +10603,7 @@
           <t>58774</t>
         </is>
       </c>
-      <c r="L18" s="6" t="inlineStr">
+      <c r="L18" s="4" t="inlineStr">
         <is>
           <t>2025-05-22 00:00:00</t>
         </is>
@@ -10456,7 +10675,7 @@
           <t>58775</t>
         </is>
       </c>
-      <c r="L19" s="6" t="inlineStr">
+      <c r="L19" s="4" t="inlineStr">
         <is>
           <t>2025-05-22 00:00:00</t>
         </is>
@@ -10471,7 +10690,7 @@
           <t>112</t>
         </is>
       </c>
-      <c r="O19" s="5" t="inlineStr">
+      <c r="O19" s="3" t="inlineStr">
         <is>
           <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\informes_tecnicos\Plan de Contingencia\VILLALBA NESTOR FABIAN\MAMPRIN Y SCEVOLA SRL</t>
         </is>

</xml_diff>

<commit_message>
mejorando la busqueda, haciendola mas veloz
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA100"/>
+  <dimension ref="A1:AA101"/>
   <sheetViews>
     <sheetView topLeftCell="G70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I102" sqref="I102"/>
@@ -9344,6 +9344,107 @@
           <t>3764251817</t>
         </is>
       </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>12/06/2025</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>MMO</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Digital</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Obra nueva</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>MENDOZA SANTIAGO</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>REDKA JAVIER</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>MARTIN FIERRO</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>191919/R/2024</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>191919</t>
+        </is>
+      </c>
+      <c r="L101" s="7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N101" s="7" t="n">
+        <v>1500</v>
+      </c>
+      <c r="O101" s="7" t="n">
+        <v>700</v>
+      </c>
+      <c r="P101" s="7" t="n">
+        <v>200</v>
+      </c>
+      <c r="Q101" t="inlineStr"/>
+      <c r="R101" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="S101" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="T101" t="inlineStr">
+        <is>
+          <t>58806</t>
+        </is>
+      </c>
+      <c r="U101" t="inlineStr">
+        <is>
+          <t>12/07/2025</t>
+        </is>
+      </c>
+      <c r="V101" t="inlineStr">
+        <is>
+          <t>MUNI DIGITAL</t>
+        </is>
+      </c>
+      <c r="W101" t="inlineStr">
+        <is>
+          <t>112</t>
+        </is>
+      </c>
+      <c r="X101" t="inlineStr">
+        <is>
+          <t>c:\Users\Admin\Desktop\Gestion-expedientes-cpim\trabajos\OBRA NUEVA\MENDOZA SANTIAGO\REDKA JAVIER</t>
+        </is>
+      </c>
+      <c r="Y101" t="inlineStr">
+        <is>
+          <t>3764251817</t>
+        </is>
+      </c>
+      <c r="Z101" t="inlineStr"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:X68"/>
@@ -11273,7 +11374,6 @@
           <t>Digital</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
           <t>Informe Técnico</t>
@@ -11302,10 +11402,6 @@
           <t>No pagado</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr">
         <is>
           <t>c:\Users\Admin\Desktop\Gestion-expedientes-cpim\informes_tecnicos\Informe Técnico\ACOSTIIITA\SANTIIII CHORI</t>
@@ -11316,7 +11412,6 @@
           <t>3764251817</t>
         </is>
       </c>
-      <c r="Q28" t="inlineStr"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
solucionando cantidad de caracteres que se pueden escribir
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA101"/>
+  <dimension ref="A1:AA109"/>
   <sheetViews>
     <sheetView topLeftCell="G70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I102" sqref="I102"/>
@@ -9403,7 +9403,6 @@
       <c r="P101" s="7" t="n">
         <v>200</v>
       </c>
-      <c r="Q101" t="inlineStr"/>
       <c r="R101" t="inlineStr">
         <is>
           <t>Pagado</t>
@@ -9444,7 +9443,527 @@
           <t>3764251817</t>
         </is>
       </c>
-      <c r="Z101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>12/06/2025</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>MMO</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Digital</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Obra nueva</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>JUANJO ROMERO</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>ORIANA MENDOZA / SANTIAGOA MENDOZA / LAUTARO MENDOZA / WALTER MENDOZA / MARIELA DIAZ MENDOZA</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>VILLA SARITA</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>12344/R/25</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>1911</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>18794</t>
+        </is>
+      </c>
+      <c r="R102" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="S102" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="X102" t="inlineStr">
+        <is>
+          <t>c:\Users\Admin\Desktop\Gestion-expedientes-cpim\trabajos\OBRA NUEVA\JUANJO ROMERO\ORIANA MENDOZA _ SANTIAGOA MENDOZA _ LAUTARO MENDOZA _ WALTER MENDOZA _ MARIELA DIAZ MENDOZA</t>
+        </is>
+      </c>
+      <c r="Y102" t="inlineStr">
+        <is>
+          <t>3764251817</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>13/06/2025</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Ingeniero</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Físico</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Registración</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>DE JESUS SANTIAGO</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>MENDOZA ORIANA / MENDOZA SANTIAGO / MENDOZA MARIELA / MENDOZA WALTER / MENDOZAAA</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>MDISDIA</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>1818/F/181</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
+      </c>
+      <c r="R103" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="S103" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>13/06/2025</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Ingeniero</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Físico</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Obra nueva</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>SANTIAGOOOOO</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>ORIANA MENDOZA / MENDOZA NOSE / MENDOZA LAUTADROOO</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>GVGERGE</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>18/R/G21</t>
+        </is>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>651</t>
+        </is>
+      </c>
+      <c r="R104" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="S104" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>13/06/2025</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Licenciado</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Físico</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Obra nueva</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>DIFI</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>FFRFERIFMERIFFERFERFGREG</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>GERGERGERG</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>188/GR/185</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>1789</t>
+        </is>
+      </c>
+      <c r="R105" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="S105" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>13/06/2025</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Licenciado</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Físico</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Obra nueva</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>LALALALALA</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>LALALA / LALALA</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>RGERGER</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>GERG/8GER</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>5145</t>
+        </is>
+      </c>
+      <c r="R106" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="S106" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>13/06/2025</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>MMO</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Físico</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Obra nueva</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>LALALAL</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>LALALA - LALALA - LALAL</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>FEWFGWEG</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>GERGV/185</t>
+        </is>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>5185</t>
+        </is>
+      </c>
+      <c r="R107" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="S107" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>13/06/2025</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Licenciado</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Físico</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Obra nueva</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>LALALALALITA</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>LALALAL - LALALALA - LALALALA - LALALALAL - LALALA</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>REGERG</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>GERGBVER/8GERERG</t>
+        </is>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>8418</t>
+        </is>
+      </c>
+      <c r="R108" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="S108" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>13/06/2025</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Licenciado</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Físico</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>178</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Obra nueva</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>benitez lucia ines</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>CARNICERIA - LA GRANKA - SIEMPRE PRECIOS BBAJOS</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>FGERWGRE</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>EWFWE/8FEW/</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr"/>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>FWEFWE</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr"/>
+      <c r="M109" t="inlineStr"/>
+      <c r="N109" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
+      <c r="P109" t="inlineStr"/>
+      <c r="Q109" t="inlineStr"/>
+      <c r="R109" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="S109" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="T109" t="inlineStr"/>
+      <c r="U109" t="inlineStr"/>
+      <c r="V109" t="inlineStr"/>
+      <c r="W109" t="inlineStr"/>
+      <c r="X109" t="inlineStr"/>
+      <c r="Y109" t="inlineStr"/>
+      <c r="Z109" t="inlineStr"/>
+      <c r="AA109" t="inlineStr"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:X68"/>

</xml_diff>